<commit_message>
Aggiunte funzionalità a SimpleGrid
</commit_message>
<xml_diff>
--- a/src/main/resources/excel/grid_output.xlsx
+++ b/src/main/resources/excel/grid_output.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="68">
   <si>
     <t>Strings Demo</t>
   </si>
@@ -38,6 +38,201 @@
   </si>
   <si>
     <t/>
+  </si>
+  <si>
+    <t>005</t>
+  </si>
+  <si>
+    <t>1,1</t>
+  </si>
+  <si>
+    <t>-1,12</t>
+  </si>
+  <si>
+    <t>-1,05</t>
+  </si>
+  <si>
+    <t>1,102</t>
+  </si>
+  <si>
+    <t>FIOGIA</t>
+  </si>
+  <si>
+    <t>01</t>
+  </si>
+  <si>
+    <t>20</t>
+  </si>
+  <si>
+    <t>001</t>
+  </si>
+  <si>
+    <t>2,0</t>
+  </si>
+  <si>
+    <t>-2,13</t>
+  </si>
+  <si>
+    <t>-2,5</t>
+  </si>
+  <si>
+    <t>2,100</t>
+  </si>
+  <si>
+    <t>SANCOS</t>
+  </si>
+  <si>
+    <t>02</t>
+  </si>
+  <si>
+    <t>33,3</t>
+  </si>
+  <si>
+    <t>3,1</t>
+  </si>
+  <si>
+    <t>-3,14</t>
+  </si>
+  <si>
+    <t>-3</t>
+  </si>
+  <si>
+    <t>-3,12541</t>
+  </si>
+  <si>
+    <t>PARFRA</t>
+  </si>
+  <si>
+    <t>03</t>
+  </si>
+  <si>
+    <t>0</t>
+  </si>
+  <si>
+    <t>002</t>
+  </si>
+  <si>
+    <t>4,2</t>
+  </si>
+  <si>
+    <t>-4,15</t>
+  </si>
+  <si>
+    <t>-4</t>
+  </si>
+  <si>
+    <t>4,40000</t>
+  </si>
+  <si>
+    <t>FORFED</t>
+  </si>
+  <si>
+    <t>12</t>
+  </si>
+  <si>
+    <t>-12,16</t>
+  </si>
+  <si>
+    <t>-12</t>
+  </si>
+  <si>
+    <t>12,12000</t>
+  </si>
+  <si>
+    <t>BELQUI</t>
+  </si>
+  <si>
+    <t>44</t>
+  </si>
+  <si>
+    <t>13,4</t>
+  </si>
+  <si>
+    <t>-13,00</t>
+  </si>
+  <si>
+    <t>-13</t>
+  </si>
+  <si>
+    <t>13.123.213,01200</t>
+  </si>
+  <si>
+    <t>ROCMAT</t>
+  </si>
+  <si>
+    <t>66</t>
+  </si>
+  <si>
+    <t>14,1</t>
+  </si>
+  <si>
+    <t>-14,01</t>
+  </si>
+  <si>
+    <t>-14</t>
+  </si>
+  <si>
+    <t>1.123.114,49000</t>
+  </si>
+  <si>
+    <t>MAEOLI</t>
+  </si>
+  <si>
+    <t>100</t>
+  </si>
+  <si>
+    <t>35,0</t>
+  </si>
+  <si>
+    <t>-35,02</t>
+  </si>
+  <si>
+    <t>-35</t>
+  </si>
+  <si>
+    <t>1.235,35900</t>
+  </si>
+  <si>
+    <t>CARLUC</t>
+  </si>
+  <si>
+    <t>1000</t>
+  </si>
+  <si>
+    <t>55</t>
+  </si>
+  <si>
+    <t>-55,03</t>
+  </si>
+  <si>
+    <t>-55</t>
+  </si>
+  <si>
+    <t>9.955,00000</t>
+  </si>
+  <si>
+    <t>CASFRA</t>
+  </si>
+  <si>
+    <t>55,22</t>
+  </si>
+  <si>
+    <t>121</t>
+  </si>
+  <si>
+    <t>-121,0</t>
+  </si>
+  <si>
+    <t>-121</t>
+  </si>
+  <si>
+    <t>121,00000</t>
+  </si>
+  <si>
+    <t>DELGIO</t>
+  </si>
+  <si>
+    <t>20,11</t>
   </si>
 </sst>
 </file>
@@ -369,7 +564,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:A3"/>
+  <dimension ref="A1:J10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="G8" sqref="G8"/>
@@ -378,6 +573,15 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" bestFit="true" customWidth="true" width="10.42578125" collapsed="false"/>
+    <col min="2" max="2" width="10.42578125" customWidth="true"/>
+    <col min="3" max="3" width="10.42578125" customWidth="true"/>
+    <col min="4" max="4" width="10.42578125" customWidth="true"/>
+    <col min="5" max="5" width="10.42578125" customWidth="true"/>
+    <col min="6" max="6" width="10.42578125" customWidth="true"/>
+    <col min="7" max="7" width="10.42578125" customWidth="true"/>
+    <col min="8" max="8" width="10.42578125" customWidth="true"/>
+    <col min="9" max="9" width="10.42578125" customWidth="true"/>
+    <col min="10" max="10" width="10.42578125" customWidth="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25" ht="15.0" customHeight="true">
@@ -386,8 +590,261 @@
       </c>
     </row>
     <row r="2" ht="15.0" customHeight="true"/>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A3" s="0"/>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25" ht="15.0" customHeight="true">
+      <c r="A3" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" t="s" s="0">
+        <v>11</v>
+      </c>
+      <c r="C3" t="s" s="0">
+        <v>11</v>
+      </c>
+      <c r="D3" t="s" s="0">
+        <v>26</v>
+      </c>
+      <c r="E3" t="s" s="0">
+        <v>26</v>
+      </c>
+      <c r="F3" t="s" s="0">
+        <v>26</v>
+      </c>
+      <c r="G3" t="s" s="0">
+        <v>26</v>
+      </c>
+      <c r="H3" t="s" s="0">
+        <v>26</v>
+      </c>
+      <c r="I3" t="s" s="0">
+        <v>11</v>
+      </c>
+      <c r="J3" t="s" s="0">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" ht="15.0" customHeight="true">
+      <c r="A4" t="s" s="0">
+        <v>4</v>
+      </c>
+      <c r="B4" t="s" s="0">
+        <v>12</v>
+      </c>
+      <c r="C4" t="s" s="0">
+        <v>19</v>
+      </c>
+      <c r="D4" t="s" s="0">
+        <v>27</v>
+      </c>
+      <c r="E4" t="s" s="0">
+        <v>32</v>
+      </c>
+      <c r="F4" t="s" s="0">
+        <v>38</v>
+      </c>
+      <c r="G4" t="s" s="0">
+        <v>44</v>
+      </c>
+      <c r="H4" t="s" s="0">
+        <v>50</v>
+      </c>
+      <c r="I4" t="s" s="0">
+        <v>56</v>
+      </c>
+      <c r="J4" t="s" s="0">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="5" ht="15.0" customHeight="true">
+      <c r="A5" t="s" s="0">
+        <v>5</v>
+      </c>
+      <c r="B5" t="s" s="0">
+        <v>13</v>
+      </c>
+      <c r="C5" t="s" s="0">
+        <v>20</v>
+      </c>
+      <c r="D5" t="s" s="0">
+        <v>28</v>
+      </c>
+      <c r="E5" t="s" s="0">
+        <v>33</v>
+      </c>
+      <c r="F5" t="s" s="0">
+        <v>39</v>
+      </c>
+      <c r="G5" t="s" s="0">
+        <v>45</v>
+      </c>
+      <c r="H5" t="s" s="0">
+        <v>51</v>
+      </c>
+      <c r="I5" t="s" s="0">
+        <v>57</v>
+      </c>
+      <c r="J5" t="s" s="0">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="6" ht="15.0" customHeight="true">
+      <c r="A6" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="B6" t="s" s="0">
+        <v>14</v>
+      </c>
+      <c r="C6" t="s" s="0">
+        <v>21</v>
+      </c>
+      <c r="D6" t="s" s="0">
+        <v>29</v>
+      </c>
+      <c r="E6" t="s" s="0">
+        <v>34</v>
+      </c>
+      <c r="F6" t="s" s="0">
+        <v>40</v>
+      </c>
+      <c r="G6" t="s" s="0">
+        <v>46</v>
+      </c>
+      <c r="H6" t="s" s="0">
+        <v>52</v>
+      </c>
+      <c r="I6" t="s" s="0">
+        <v>58</v>
+      </c>
+      <c r="J6" t="s" s="0">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="7" ht="15.0" customHeight="true">
+      <c r="A7" t="s" s="0">
+        <v>7</v>
+      </c>
+      <c r="B7" t="s" s="0">
+        <v>15</v>
+      </c>
+      <c r="C7" t="s" s="0">
+        <v>22</v>
+      </c>
+      <c r="D7" t="s" s="0">
+        <v>30</v>
+      </c>
+      <c r="E7" t="s" s="0">
+        <v>35</v>
+      </c>
+      <c r="F7" t="s" s="0">
+        <v>41</v>
+      </c>
+      <c r="G7" t="s" s="0">
+        <v>47</v>
+      </c>
+      <c r="H7" t="s" s="0">
+        <v>53</v>
+      </c>
+      <c r="I7" t="s" s="0">
+        <v>59</v>
+      </c>
+      <c r="J7" t="s" s="0">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="8" ht="15.0" customHeight="true">
+      <c r="A8" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="B8" t="s" s="0">
+        <v>16</v>
+      </c>
+      <c r="C8" t="s" s="0">
+        <v>23</v>
+      </c>
+      <c r="D8" t="s" s="0">
+        <v>31</v>
+      </c>
+      <c r="E8" t="s" s="0">
+        <v>36</v>
+      </c>
+      <c r="F8" t="s" s="0">
+        <v>42</v>
+      </c>
+      <c r="G8" t="s" s="0">
+        <v>48</v>
+      </c>
+      <c r="H8" t="s" s="0">
+        <v>54</v>
+      </c>
+      <c r="I8" t="s" s="0">
+        <v>60</v>
+      </c>
+      <c r="J8" t="s" s="0">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="9" ht="15.0" customHeight="true">
+      <c r="A9" t="s" s="0">
+        <v>9</v>
+      </c>
+      <c r="B9" t="s" s="0">
+        <v>17</v>
+      </c>
+      <c r="C9" t="s" s="0">
+        <v>24</v>
+      </c>
+      <c r="D9" t="s" s="0">
+        <v>9</v>
+      </c>
+      <c r="E9" t="s" s="0">
+        <v>9</v>
+      </c>
+      <c r="F9" t="s" s="0">
+        <v>9</v>
+      </c>
+      <c r="G9" t="s" s="0">
+        <v>9</v>
+      </c>
+      <c r="H9" t="s" s="0">
+        <v>9</v>
+      </c>
+      <c r="I9" t="s" s="0">
+        <v>9</v>
+      </c>
+      <c r="J9" t="s" s="0">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="10" ht="15.0" customHeight="true">
+      <c r="A10" t="s" s="0">
+        <v>10</v>
+      </c>
+      <c r="B10" t="s" s="0">
+        <v>18</v>
+      </c>
+      <c r="C10" t="s" s="0">
+        <v>25</v>
+      </c>
+      <c r="D10" t="s" s="0">
+        <v>25</v>
+      </c>
+      <c r="E10" t="s" s="0">
+        <v>37</v>
+      </c>
+      <c r="F10" t="s" s="0">
+        <v>43</v>
+      </c>
+      <c r="G10" t="s" s="0">
+        <v>49</v>
+      </c>
+      <c r="H10" t="s" s="0">
+        <v>55</v>
+      </c>
+      <c r="I10" t="s" s="0">
+        <v>61</v>
+      </c>
+      <c r="J10" t="s" s="0">
+        <v>67</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>